<commit_message>
duplication & similarity checking completed
</commit_message>
<xml_diff>
--- a/QuestionBank-Template-V1_duplicateQ.xlsx
+++ b/QuestionBank-Template-V1_duplicateQ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bella\Desktop\SeniorProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39CBAB6-B9B6-462C-A822-F57D41F381AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0E6B4D-EFC3-436D-AA02-BBCA2B1E03EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="118">
   <si>
     <t>T</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t>Beef Jerky</t>
+  </si>
+  <si>
+    <t>Which one is a mammal?</t>
   </si>
 </sst>
 </file>
@@ -804,7 +807,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45888</v>
+        <v>45895</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1037,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3C1A04-8C9A-4AB3-92D4-9CFE7C63CA0B}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,6 +1284,35 @@
         <v>32</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1291,7 +1323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589423D0-50CB-4F3F-82F4-CB353E932D78}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>